<commit_message>
Add 4 letter word lists
</commit_message>
<xml_diff>
--- a/experiment/RUN_ME/stimuli/word_lists/word_freq_list.xlsx
+++ b/experiment/RUN_ME/stimuli/word_lists/word_freq_list.xlsx
@@ -1,24 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\university\mudrick_lab\subliminal_priming_w_motion_capture\experiment\RUN_ME\stimuli\word_lists\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{254BFC77-12E2-49B4-AD62-75CE1F77E75F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F60B561D-3F06-46AB-B61E-53CF1699CF58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="24432" yWindow="10104" windowWidth="18900" windowHeight="11052" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -368,7 +377,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:D31" totalsRowShown="0" headerRowDxfId="2" tableBorderDxfId="1">
   <autoFilter ref="A1:D31" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D31">
-    <sortCondition ref="A1:A31"/>
+    <sortCondition ref="D1:D31"/>
   </sortState>
   <tableColumns count="4">
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="natural" dataDxfId="0"/>
@@ -645,7 +654,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H46"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A5" workbookViewId="0">
       <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
@@ -676,255 +685,255 @@
       <c r="H1" s="1"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>8</v>
+      <c r="A2" s="4" t="s">
+        <v>41</v>
       </c>
       <c r="B2" s="3">
-        <v>23</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" s="3">
-        <v>14</v>
+        <v>18</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="D2">
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="B3" s="3">
-        <v>45</v>
+        <v>63</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="D3" s="3">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B4" s="3">
-        <v>28</v>
+        <v>51</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="D4" s="3">
-        <v>30</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
-        <v>41</v>
+        <v>57</v>
       </c>
       <c r="B5" s="3">
-        <v>18</v>
+        <v>35</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="D5">
-        <v>10</v>
+        <v>34</v>
+      </c>
+      <c r="D5" s="3">
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="B6" s="3">
-        <v>12</v>
-      </c>
-      <c r="C6" t="s">
-        <v>53</v>
+        <v>23</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>3</v>
       </c>
       <c r="D6" s="3">
-        <v>38</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="B7">
-        <v>52</v>
+        <v>27</v>
+      </c>
+      <c r="B7" s="3">
+        <v>45</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="D7" s="3">
-        <v>21</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B8" s="3">
-        <v>51</v>
+        <v>52</v>
+      </c>
+      <c r="B8">
+        <v>38</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D8" s="3">
-        <v>12</v>
+        <v>33</v>
+      </c>
+      <c r="D8">
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>23</v>
+        <v>47</v>
       </c>
       <c r="B9" s="3">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>2</v>
+        <v>49</v>
       </c>
       <c r="D9" s="3">
-        <v>32</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A10" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B10" s="3">
-        <v>11</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>14</v>
+      <c r="A10" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B10" s="9">
+        <v>88</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>58</v>
       </c>
       <c r="D10" s="3">
-        <v>41</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A11" s="4" t="s">
-        <v>43</v>
+      <c r="A11" s="2" t="s">
+        <v>21</v>
       </c>
       <c r="B11" s="3">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>37</v>
+        <v>4</v>
       </c>
       <c r="D11" s="3">
-        <v>36</v>
+        <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B12">
+        <v>52</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12" s="3">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B13" s="3">
+        <v>113</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D13" s="3">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="B12" s="3">
+      <c r="B14" s="3">
         <v>18</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C14" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D12" s="3">
+      <c r="D14" s="3">
         <v>22</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A13" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="B13" s="3">
-        <v>36</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="D13" s="3">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A14" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="B14" s="3">
-        <v>17</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="D14">
-        <v>26</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B15" s="3">
+        <v>36</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D15" s="3">
         <v>24</v>
       </c>
-      <c r="C15" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="D15" s="3">
-        <v>39</v>
-      </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A16" s="4" t="s">
-        <v>57</v>
+      <c r="A16" s="2" t="s">
+        <v>9</v>
       </c>
       <c r="B16" s="3">
-        <v>35</v>
-      </c>
-      <c r="C16" s="6" t="s">
-        <v>34</v>
+        <v>17</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>62</v>
       </c>
       <c r="D16" s="3">
-        <v>12</v>
+        <v>25</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" s="3" t="s">
+      <c r="A17" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B17" s="3">
+        <v>17</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D17">
         <v>26</v>
-      </c>
-      <c r="B17" s="3">
-        <v>16</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D17" s="3">
-        <v>40</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B18" s="3">
         <v>40</v>
       </c>
-      <c r="B18" s="3">
+      <c r="C18" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="D18" s="3">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B19" s="3">
+        <v>28</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D19" s="3">
         <v>30</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="D18">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="B19" s="3">
-        <v>65</v>
-      </c>
-      <c r="C19" t="s">
-        <v>50</v>
-      </c>
-      <c r="D19" s="3">
-        <v>35</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
@@ -942,157 +951,157 @@
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" s="4" t="s">
-        <v>63</v>
+      <c r="A21" s="2" t="s">
+        <v>23</v>
       </c>
       <c r="B21" s="3">
-        <v>16</v>
+        <v>36</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>28</v>
+        <v>2</v>
       </c>
       <c r="D21" s="5">
-        <v>63</v>
+        <v>32</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" s="2" t="s">
-        <v>54</v>
+      <c r="A22" s="4" t="s">
+        <v>59</v>
       </c>
       <c r="B22" s="3">
-        <v>113</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>5</v>
+        <v>65</v>
+      </c>
+      <c r="C22" t="s">
+        <v>50</v>
       </c>
       <c r="D22" s="3">
-        <v>21</v>
+        <v>35</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23" s="2" t="s">
+      <c r="A23" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B23" s="3">
         <v>13</v>
       </c>
-      <c r="B23" s="3">
-        <v>63</v>
-      </c>
       <c r="C23" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D23" s="3">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B24" s="3">
         <v>12</v>
       </c>
-      <c r="D23" s="3">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="B24" s="9">
-        <v>88</v>
-      </c>
-      <c r="C24" s="6" t="s">
-        <v>58</v>
+      <c r="C24" t="s">
+        <v>53</v>
       </c>
       <c r="D24" s="3">
-        <v>18</v>
+        <v>38</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="s">
-        <v>61</v>
+        <v>40</v>
       </c>
       <c r="B25" s="3">
-        <v>77</v>
+        <v>30</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D25" s="3">
-        <v>69</v>
+        <v>35</v>
+      </c>
+      <c r="D25">
+        <v>38</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A26" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="B26">
-        <v>38</v>
+      <c r="A26" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B26" s="3">
+        <v>24</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="D26">
-        <v>17</v>
+        <v>55</v>
+      </c>
+      <c r="D26" s="3">
+        <v>39</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
-        <v>1</v>
+        <v>26</v>
       </c>
       <c r="B27" s="3">
-        <v>55</v>
+        <v>16</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="D27" s="3">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="B28" s="3">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>62</v>
+        <v>14</v>
       </c>
       <c r="D28" s="3">
-        <v>25</v>
+        <v>41</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
-        <v>21</v>
+        <v>1</v>
       </c>
       <c r="B29" s="3">
-        <v>22</v>
+        <v>55</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="D29" s="3">
-        <v>18</v>
+        <v>41</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A30" s="2" t="s">
-        <v>47</v>
+      <c r="A30" s="4" t="s">
+        <v>63</v>
       </c>
       <c r="B30" s="3">
-        <v>38</v>
+        <v>16</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>49</v>
+        <v>28</v>
       </c>
       <c r="D30" s="3">
-        <v>17</v>
+        <v>63</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" s="4" t="s">
-        <v>38</v>
+        <v>61</v>
       </c>
       <c r="B31" s="3">
-        <v>40</v>
-      </c>
-      <c r="C31" s="6" t="s">
-        <v>56</v>
+        <v>77</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>15</v>
       </c>
       <c r="D31" s="3">
-        <v>29</v>
+        <v>69</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="15" x14ac:dyDescent="0.25">

</xml_diff>